<commit_message>
some code cleanup and adding documentation
</commit_message>
<xml_diff>
--- a/testData/annotatedTestBean.xlsx
+++ b/testData/annotatedTestBean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\LightweightFileObjectIO\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\MikeBeanUtils\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AAAF8B-D46C-4DE9-88D2-51E23859037D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E9BE57-38C3-4319-8789-55893526F575}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42520" yWindow="4120" windowWidth="14600" windowHeight="6230" xr2:uid="{178436EE-5940-45E8-83F9-D293550344BB}"/>
+    <workbookView xWindow="1098" yWindow="1098" windowWidth="17280" windowHeight="8994" xr2:uid="{178436EE-5940-45E8-83F9-D293550344BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>iSt</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>S;L</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>d2</t>
   </si>
 </sst>
 </file>
@@ -442,15 +448,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E54B1-A21F-459F-84AD-E615CE18CC5D}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="M1" sqref="M1:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,8 +493,14 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>-12345</v>
       </c>
@@ -525,8 +537,14 @@
       <c r="L2" t="s">
         <v>9</v>
       </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>-12345</v>
       </c>
@@ -563,8 +581,14 @@
       <c r="L3" t="s">
         <v>9</v>
       </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>-12345</v>
       </c>
@@ -601,8 +625,14 @@
       <c r="L4" t="s">
         <v>9</v>
       </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>-12345</v>
       </c>
@@ -639,8 +669,14 @@
       <c r="L5" t="s">
         <v>9</v>
       </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>-12345</v>
       </c>
@@ -676,6 +712,12 @@
       </c>
       <c r="L6" t="s">
         <v>9</v>
+      </c>
+      <c r="M6">
+        <v>7</v>
+      </c>
+      <c r="N6">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>